<commit_message>
Add features, update dictionary
</commit_message>
<xml_diff>
--- a/reports/data_dictionary.xlsx
+++ b/reports/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Documents/phd/projects/tcors_ub/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E8EC72-FED0-5442-864C-F7D51B2DB0D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B2FBBC-6DD1-1D43-A00E-9C8FC757679C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{BACE2C31-F40C-A84A-9700-D57383A4DEAB}"/>
+    <workbookView xWindow="41520" yWindow="-240" windowWidth="28040" windowHeight="17440" xr2:uid="{BACE2C31-F40C-A84A-9700-D57383A4DEAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
   <si>
     <t>screen_id</t>
   </si>
@@ -218,6 +218,36 @@
   </si>
   <si>
     <t>proprtion of total cigarettes that were study-provided (study_mean / total_cpd)</t>
+  </si>
+  <si>
+    <t>total_cpd_bin</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>original</t>
+  </si>
+  <si>
+    <t>external</t>
+  </si>
+  <si>
+    <t>calculated</t>
+  </si>
+  <si>
+    <t>total_cpd binned into intervals of 5cpd up to 80cpd (i.e., the final bin is 80 to infinity)</t>
+  </si>
+  <si>
+    <t>cpd_bin_label</t>
+  </si>
+  <si>
+    <t>sequential label of total_cpd_bin</t>
+  </si>
+  <si>
+    <t>prp_change</t>
+  </si>
+  <si>
+    <t>ratio of total_cpd / baseline_cpd. If total_cpd = 0, prp_change = -1</t>
   </si>
 </sst>
 </file>
@@ -584,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81492DA7-182B-9E46-A20C-686CC65EBF0F}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -607,6 +637,9 @@
       <c r="C1" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -618,7 +651,9 @@
       <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -630,6 +665,9 @@
       <c r="C3" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -641,6 +679,9 @@
       <c r="C4" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -652,6 +693,9 @@
       <c r="C5" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="D5" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -663,6 +707,9 @@
       <c r="C6" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="D6" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -674,6 +721,9 @@
       <c r="C7" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="D7" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -685,6 +735,9 @@
       <c r="C8" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="D8" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -696,6 +749,9 @@
       <c r="C9" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="D9" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -707,6 +763,9 @@
       <c r="C10" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -718,6 +777,9 @@
       <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="D11" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -729,6 +791,9 @@
       <c r="C12" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="D12" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -740,6 +805,9 @@
       <c r="C13" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="D13" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -751,6 +819,9 @@
       <c r="C14" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="D14" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
@@ -762,6 +833,9 @@
       <c r="C15" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="D15" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -773,8 +847,11 @@
       <c r="C16" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="D16" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -784,8 +861,11 @@
       <c r="C17" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D17" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -794,6 +874,51 @@
       </c>
       <c r="C18" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>